<commit_message>
todos los cambios a orderby y generando reportes ordenados por vacantes
</commit_message>
<xml_diff>
--- a/vaca.xlsx
+++ b/vaca.xlsx
@@ -14,9 +14,123 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>CEPU</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+  <si>
+    <t>ADMINISTRACIÓN</t>
+  </si>
+  <si>
+    <t>AGRONOMÍA</t>
+  </si>
+  <si>
+    <t>ARQUITECTURA</t>
+  </si>
+  <si>
+    <t>FÍSICA</t>
+  </si>
+  <si>
+    <t>ESTADÍSTICA</t>
+  </si>
+  <si>
+    <t>MATEMÁTICA E INFORMÁTICA</t>
+  </si>
+  <si>
+    <t>BIOLOGÍA</t>
+  </si>
+  <si>
+    <t>CIENCIAS DE LA COMUNICACIÓN</t>
+  </si>
+  <si>
+    <t>TURISMO</t>
+  </si>
+  <si>
+    <t>ARQUEOLOGÍA</t>
+  </si>
+  <si>
+    <t>ECONOMÍA</t>
+  </si>
+  <si>
+    <t>NEGOCIOS INTERNACIONALES</t>
+  </si>
+  <si>
+    <t>CIENCIAS DE LA EDUCACIÓN EN LENGUA Y LITERATURA</t>
+  </si>
+  <si>
+    <t>CIENCIAS DE LA EDUCACIÓN EN HISTORIA Y GEOGRAFÍA</t>
+  </si>
+  <si>
+    <t>CIENCIAS DE LA EDUCACIÓN EN FILOSOFÍA, PSICOLOGÍA Y CIENCIAS SOCIALES</t>
+  </si>
+  <si>
+    <t>CIENCIAS DE LA EDUCACIÓN EN CIENCIAS BIOLÓGICAS Y QUÍMICA</t>
+  </si>
+  <si>
+    <t>CIENCIAS DE LA EDUCACIÓN EN MATEMÁTICA E INFORMÁTICA</t>
+  </si>
+  <si>
+    <t>CIENCIAS DE LA EDUCACIÓN EN EDUCACIÓN INICIAL</t>
+  </si>
+  <si>
+    <t>CIENCIAS DE LA EDUCACIÓN EN EDUCACIÓN PRIMARIA</t>
+  </si>
+  <si>
+    <t>CIENCIAS DE LA EDUCACIÓN EN EDUCACIÓN ARTÍSTICA</t>
+  </si>
+  <si>
+    <t>CIENCIAS DE LA EDUCACIÓN EN EDUCACIÓN FÍSICA</t>
+  </si>
+  <si>
+    <t>CONTABILIDAD</t>
+  </si>
+  <si>
+    <t>DERECHO</t>
+  </si>
+  <si>
+    <t>ENFERMERÍA</t>
+  </si>
+  <si>
+    <t>FARMACIA Y BIOQUÍMICA</t>
+  </si>
+  <si>
+    <t>INGENIERÍA AMBIENTAL Y SANITARIA</t>
+  </si>
+  <si>
+    <t>INGENIERÍA CIVIL</t>
+  </si>
+  <si>
+    <t>INGENIERÍA ELECTRÓNICA</t>
+  </si>
+  <si>
+    <t>INGENIERÍA MECÁNICA ELÉCTRICA</t>
+  </si>
+  <si>
+    <t>INGENIERÍA DE MINAS</t>
+  </si>
+  <si>
+    <t>INGENIERÍA METALÚRGICA</t>
+  </si>
+  <si>
+    <t>INGENIERÍA PESQUERA</t>
+  </si>
+  <si>
+    <t>INGENIERÍA DE ALIMENTOS</t>
+  </si>
+  <si>
+    <t>INGENIERÍA QUÍMICA</t>
+  </si>
+  <si>
+    <t>INGENIERÍA DE SISTEMAS</t>
+  </si>
+  <si>
+    <t>MEDICINA VETERINARIA Y ZOOTECNIA</t>
+  </si>
+  <si>
+    <t>OBSTETRICIA</t>
+  </si>
+  <si>
+    <t>ODONTOLOGÍA</t>
+  </si>
+  <si>
+    <t>PSICOLOGÍA</t>
   </si>
 </sst>
 </file>
@@ -24,20 +138,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -59,23 +166,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -119,19 +215,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -438,212 +537,325 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A40"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="44.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2">
+        <v>38</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+      <c r="A26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3">
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+      <c r="A27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+      <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+      <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="2">
+      <c r="B32" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
+      <c r="A33" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
+      <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
+      <c r="A35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3">
+        <v>26</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
+      <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="3">
-        <v>23</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="2">
-        <v>21</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="3">
-        <v>21</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="2">
-        <v>21</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="3">
-        <v>21</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="2">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="3">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="3">
-        <v>43</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
-      <c r="A24" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
-      <c r="A25" s="3">
+      <c r="B37" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
+      <c r="A38" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3">
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
-      <c r="A26" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
-      <c r="A27" s="3">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
+      <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
-      <c r="A28" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
-      <c r="A29" s="3">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
-      <c r="A30" s="2">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
-      <c r="A31" s="3">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
-      <c r="A32" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
-      <c r="A33" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
-      <c r="A34" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
-      <c r="A35" s="3">
-        <v>28</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
-      <c r="A36" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
-      <c r="A37" s="3">
-        <v>26</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
-      <c r="A38" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
-      <c r="A39" s="3">
-        <v>24</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
-      <c r="A40" s="4">
+      <c r="B39" s="4">
         <v>11</v>
       </c>
     </row>

</xml_diff>